<commit_message>
Foi ajustado os dias de cada sprint.
</commit_message>
<xml_diff>
--- a/Organização das sprints.xlsx
+++ b/Organização das sprints.xlsx
@@ -378,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -398,9 +398,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -434,10 +435,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,7 +742,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,16 +754,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -786,7 +783,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="21" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -811,10 +808,12 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="30">
+      <c r="G3" s="33">
         <v>42120</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="33">
+        <v>42131</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -834,8 +833,8 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -855,8 +854,8 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -868,8 +867,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -881,23 +880,23 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -912,12 +911,12 @@
       <c r="C9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="20" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="22" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="10" t="s">
@@ -942,8 +941,12 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="G10" s="33">
+        <v>42132</v>
+      </c>
+      <c r="H10" s="33">
+        <v>42143</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -963,8 +966,8 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -984,8 +987,8 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -997,8 +1000,8 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1010,8 +1013,8 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1023,23 +1026,23 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="32"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -1057,7 +1060,7 @@
       <c r="D17" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1092,8 +1095,12 @@
       <c r="F18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="G18" s="33">
+        <v>42144</v>
+      </c>
+      <c r="H18" s="33">
+        <v>42155</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1117,8 +1124,8 @@
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1142,8 +1149,8 @@
       <c r="F20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1155,8 +1162,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
       <c r="I21" s="4" t="s">
         <v>12</v>
       </c>
@@ -1170,8 +1177,8 @@
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1183,8 +1190,8 @@
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>

</xml_diff>

<commit_message>
Foi mudado a abordagem do sistema.
</commit_message>
<xml_diff>
--- a/Organização das sprints.xlsx
+++ b/Organização das sprints.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\system_far\controle_estique\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -35,9 +30,6 @@
     <t>Cadastro cliente</t>
   </si>
   <si>
-    <t>Cadastro Fornecedor</t>
-  </si>
-  <si>
     <t>Mockaps</t>
   </si>
   <si>
@@ -96,6 +88,9 @@
   </si>
   <si>
     <t>natan</t>
+  </si>
+  <si>
+    <t>Cadastro de ordem de serviço</t>
   </si>
 </sst>
 </file>
@@ -402,6 +397,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -431,9 +429,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -495,7 +490,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,7 +525,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -742,28 +737,29 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="6" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="6" width="20.42578125" customWidth="1"/>
     <col min="7" max="7" width="10.140625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -773,21 +769,21 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -795,23 +791,23 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="33">
+      <c r="G3" s="23">
         <v>42120</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="23">
         <v>42131</v>
       </c>
       <c r="I3" s="4"/>
@@ -820,42 +816,42 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -867,8 +863,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -880,47 +876,47 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>9</v>
-      </c>
       <c r="D9" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -928,23 +924,23 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="33">
+      <c r="G10" s="23">
         <v>42132</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="23">
         <v>42143</v>
       </c>
       <c r="I10" s="4"/>
@@ -953,42 +949,42 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1000,8 +996,8 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1013,8 +1009,8 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1026,51 +1022,51 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="D17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="15" t="s">
+      <c r="H17" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1078,27 +1074,27 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="33">
+        <v>22</v>
+      </c>
+      <c r="G18" s="23">
         <v>42144</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="23">
         <v>42155</v>
       </c>
       <c r="I18" s="4"/>
@@ -1107,50 +1103,50 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+        <v>13</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+        <v>23</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1162,10 +1158,10 @@
       <c r="D21" s="1"/>
       <c r="E21" s="7"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
       <c r="I21" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1177,8 +1173,8 @@
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1190,8 +1186,8 @@
       <c r="D23" s="1"/>
       <c r="E23" s="7"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>

</xml_diff>

<commit_message>
Sistema em fasse de criação
</commit_message>
<xml_diff>
--- a/Organização das sprints.xlsx
+++ b/Organização das sprints.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -84,7 +85,7 @@
     <t>Serviços abertos</t>
   </si>
   <si>
-    <t>Serviços em realizados</t>
+    <t>Serviços realizados</t>
   </si>
 </sst>
 </file>
@@ -407,6 +408,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,34 +430,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,6 +446,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -763,7 +764,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,39 +777,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="4"/>
@@ -816,13 +817,13 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -830,10 +831,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="9">
+      <c r="G3" s="22">
         <v>42120</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="22">
         <v>42131</v>
       </c>
       <c r="I3" s="4"/>
@@ -841,13 +842,13 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -855,20 +856,20 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -876,72 +877,72 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="17"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="17"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="16" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="4"/>
@@ -949,13 +950,13 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -963,10 +964,10 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="9">
+      <c r="G10" s="22">
         <v>42132</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="22">
         <v>42143</v>
       </c>
       <c r="I10" s="4"/>
@@ -974,13 +975,13 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -988,20 +989,20 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1009,87 +1010,87 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="17" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="4"/>
@@ -1097,13 +1098,13 @@
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1113,10 +1114,10 @@
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="22">
         <v>42144</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="22">
         <v>42155</v>
       </c>
       <c r="I18" s="4"/>
@@ -1124,13 +1125,13 @@
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1140,20 +1141,20 @@
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1163,21 +1164,21 @@
       <c r="F20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="17"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="1"/>
       <c r="E21" s="6"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
       <c r="I21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1185,27 +1186,27 @@
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="17"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="1"/>
       <c r="E22" s="6"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="17"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="1"/>
       <c r="E23" s="6"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>

</xml_diff>

<commit_message>
Foi terminado o sistema.
</commit_message>
<xml_diff>
--- a/Organização das sprints.xlsx
+++ b/Organização das sprints.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -64,18 +63,9 @@
     <t>Ruan</t>
   </si>
   <si>
-    <t>Relatório</t>
-  </si>
-  <si>
     <t>Responsável</t>
   </si>
   <si>
-    <t>vinícius</t>
-  </si>
-  <si>
-    <t>natan</t>
-  </si>
-  <si>
     <t>Cadastro de ordem de serviço</t>
   </si>
   <si>
@@ -86,13 +76,19 @@
   </si>
   <si>
     <t>Serviços realizados</t>
+  </si>
+  <si>
+    <t>Clientes Cadastrados</t>
+  </si>
+  <si>
+    <t>Funcionários Cadastrados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +100,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -398,29 +387,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -430,32 +416,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,7 +753,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,39 +766,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>16</v>
+      <c r="B2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="4"/>
@@ -817,13 +806,13 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -831,10 +820,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="22">
+      <c r="G3" s="19">
         <v>42120</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="19">
         <v>42131</v>
       </c>
       <c r="I3" s="4"/>
@@ -842,13 +831,13 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -856,20 +845,20 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -877,72 +866,72 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="14"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="14"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>16</v>
+      <c r="D9" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="I9" s="4"/>
@@ -950,13 +939,13 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -964,10 +953,10 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="22">
+      <c r="G10" s="19">
         <v>42132</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="19">
         <v>42143</v>
       </c>
       <c r="I10" s="4"/>
@@ -975,13 +964,13 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -989,20 +978,20 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1010,87 +999,89 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="14"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="14"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="14"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="21" t="s">
+      <c r="C17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="4"/>
@@ -1098,26 +1089,28 @@
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="22">
+        <v>8</v>
+      </c>
+      <c r="G18" s="19">
         <v>42144</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="19">
         <v>42155</v>
       </c>
       <c r="I18" s="4"/>
@@ -1125,60 +1118,64 @@
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="11" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
+        <v>14</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="14"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1186,27 +1183,27 @@
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="14"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="14"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>

</xml_diff>

<commit_message>
Alterações nas prioridades das sprints
</commit_message>
<xml_diff>
--- a/Organização das sprints.xlsx
+++ b/Organização das sprints.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -407,6 +407,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -442,9 +445,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,7 +753,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,16 +766,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -820,10 +820,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="19">
+      <c r="G3" s="20">
         <v>42120</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="20">
         <v>42131</v>
       </c>
       <c r="I3" s="4"/>
@@ -845,8 +845,8 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -866,8 +866,8 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -879,8 +879,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -892,23 +892,23 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -926,8 +926,12 @@
       <c r="D9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>15</v>
+      </c>
       <c r="G9" s="16" t="s">
         <v>11</v>
       </c>
@@ -951,12 +955,16 @@
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="19">
+      <c r="E10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="20">
         <v>42132</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H10" s="20">
         <v>42143</v>
       </c>
       <c r="I10" s="4"/>
@@ -976,10 +984,14 @@
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="E11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -997,10 +1009,14 @@
       <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="E12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1010,10 +1026,10 @@
       <c r="B13" s="1"/>
       <c r="C13" s="11"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1023,10 +1039,10 @@
       <c r="B14" s="1"/>
       <c r="C14" s="11"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1036,25 +1052,25 @@
       <c r="B15" s="1"/>
       <c r="C15" s="11"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
@@ -1072,7 +1088,7 @@
       <c r="D17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="12" t="s">
@@ -1107,10 +1123,10 @@
       <c r="F18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="20">
         <v>42144</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="20">
         <v>42155</v>
       </c>
       <c r="I18" s="4"/>
@@ -1136,8 +1152,8 @@
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1161,8 +1177,8 @@
       <c r="F20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1174,8 +1190,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="11"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1189,8 +1205,8 @@
       <c r="D22" s="1"/>
       <c r="E22" s="11"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1202,8 +1218,8 @@
       <c r="D23" s="1"/>
       <c r="E23" s="11"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>

</xml_diff>